<commit_message>
addin all data based color genetic for head adding calculated option
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yossi\source\repos\yossiii050\FeatherFriend\DataBased\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7AC9C0E-1B18-4FCA-A568-3AD34705D9C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7F841D0-7E5B-432B-B6D7-46A2D327837F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5352" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1065" yWindow="4965" windowWidth="18855" windowHeight="16035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
   <si>
     <t>CageID</t>
   </si>
@@ -60,12 +60,6 @@
     <t>BreastColor</t>
   </si>
   <si>
-    <t>ggg</t>
-  </si>
-  <si>
-    <t>uuu</t>
-  </si>
-  <si>
     <t>12A</t>
   </si>
   <si>
@@ -73,6 +67,45 @@
   </si>
   <si>
     <t>יום שני 15 מאי 2023</t>
+  </si>
+  <si>
+    <t>Female</t>
+  </si>
+  <si>
+    <t>European Gouldian</t>
+  </si>
+  <si>
+    <t>East Europe</t>
+  </si>
+  <si>
+    <t>Australian Gouldian</t>
+  </si>
+  <si>
+    <t>Coastal Cities</t>
+  </si>
+  <si>
+    <t>American Gouldian</t>
+  </si>
+  <si>
+    <t>North America</t>
+  </si>
+  <si>
+    <t>Red</t>
+  </si>
+  <si>
+    <t>50A</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>12B</t>
+  </si>
+  <si>
+    <t>13A</t>
+  </si>
+  <si>
+    <t>15A</t>
   </si>
 </sst>
 </file>
@@ -108,8 +141,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -390,64 +429,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="A2:F6"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
+    <col min="9" max="9" width="12.125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>111</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -456,7 +500,392 @@
         <v>99</v>
       </c>
       <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>223</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>99</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>22</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="2">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>223</v>
+      </c>
+      <c r="G4">
+        <v>111</v>
+      </c>
+      <c r="H4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>196</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5">
+        <v>23</v>
+      </c>
+      <c r="G5">
+        <v>22</v>
+      </c>
+      <c r="H5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>54</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="2">
+        <v>444</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>223</v>
+      </c>
+      <c r="G6">
+        <v>123</v>
+      </c>
+      <c r="H6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>55</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="2">
+        <v>1111</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>196</v>
+      </c>
+      <c r="G7">
+        <v>111</v>
+      </c>
+      <c r="H7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>845</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="2">
+        <v>444</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>23</v>
+      </c>
+      <c r="G8">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>239</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="2">
+        <v>11</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>23</v>
+      </c>
+      <c r="G9">
+        <v>111</v>
+      </c>
+      <c r="H9" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>2053</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>223</v>
+      </c>
+      <c r="G10">
+        <v>111</v>
+      </c>
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>5436</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11">
+        <v>223</v>
+      </c>
+      <c r="G11">
+        <v>111</v>
+      </c>
+      <c r="H11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>4321</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="2">
+        <v>444</v>
+      </c>
+      <c r="E12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12">
+        <v>223</v>
+      </c>
+      <c r="G12">
+        <v>111</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>5032</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13">
+        <v>223</v>
+      </c>
+      <c r="G13">
+        <v>111</v>
+      </c>
+      <c r="H13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>1412</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="2">
+        <v>11</v>
+      </c>
+      <c r="E14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14">
+        <v>223</v>
+      </c>
+      <c r="G14">
+        <v>111</v>
+      </c>
+      <c r="H14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>4324</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15">
+        <v>223</v>
+      </c>
+      <c r="G15">
+        <v>111</v>
+      </c>
+      <c r="H15" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>121612</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16">
+        <v>223</v>
+      </c>
+      <c r="G16">
+        <v>111</v>
+      </c>
+      <c r="H16" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding ID to register page
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6902FF0E-1784-4659-97EF-BB3379AB5BB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BCAD7A-BE81-41AA-8132-0DA47B46B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="11520" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
   <si>
     <t>CageID</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>15A</t>
+  </si>
+  <si>
+    <t>Australian Gouldian</t>
+  </si>
+  <si>
+    <t>Coastal Cities</t>
   </si>
 </sst>
 </file>
@@ -742,27 +748,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.59765625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.8984375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -797,7 +803,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>111</v>
       </c>
@@ -832,7 +838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>223</v>
       </c>
@@ -867,7 +873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1231</v>
       </c>
@@ -902,7 +908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>435345</v>
       </c>
@@ -937,7 +943,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>534534</v>
       </c>
@@ -969,7 +975,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>432423</v>
       </c>
@@ -1002,6 +1008,41 @@
       </c>
       <c r="K7" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8">
+        <v>223</v>
+      </c>
+      <c r="G8">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added cage and bird info includes update information
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100955A0-AEFE-4AB1-BE3B-1E0670294935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC23F789-E83C-4273-A330-364B1FA78B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1740" yWindow="0" windowWidth="11520" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2088" yWindow="0" windowWidth="11520" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t>CageID</t>
   </si>
@@ -105,16 +105,16 @@
     <t>Pastel</t>
   </si>
   <si>
-    <t>50A</t>
-  </si>
-  <si>
     <t>15A</t>
   </si>
   <si>
-    <t>Western Europe</t>
-  </si>
-  <si>
-    <t>Blue</t>
+    <t>Australian Gouldian</t>
+  </si>
+  <si>
+    <t>Coastal Cities</t>
+  </si>
+  <si>
+    <t>13A</t>
   </si>
 </sst>
 </file>
@@ -748,15 +748,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.8984375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
@@ -919,7 +919,7 @@
         <v>17</v>
       </c>
       <c r="D5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>
@@ -989,7 +989,7 @@
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>12</v>
@@ -1015,16 +1015,16 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>12341234</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="C8" t="s">
         <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="E8" t="s">
         <v>13</v>
@@ -1033,54 +1033,19 @@
         <v>223</v>
       </c>
       <c r="G8">
-        <v>435345</v>
-      </c>
-      <c r="H8" s="3">
-        <v>44930</v>
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
         <v>20</v>
       </c>
       <c r="K8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2580</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9">
-        <v>12341234</v>
-      </c>
-      <c r="G9">
-        <v>111</v>
-      </c>
-      <c r="H9" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" t="s">
-        <v>20</v>
-      </c>
-      <c r="K9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit changes before pull
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6BCAD7A-BE81-41AA-8132-0DA47B46B60C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF6B6AC-CA57-4A74-9C1D-D26686C65A62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="72" yWindow="336" windowWidth="11976" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
   <si>
     <t>CageID</t>
   </si>
@@ -115,6 +115,12 @@
   </si>
   <si>
     <t>Coastal Cities</t>
+  </si>
+  <si>
+    <t>Western Europe</t>
+  </si>
+  <si>
+    <t>Central America</t>
   </si>
 </sst>
 </file>
@@ -748,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -974,6 +980,9 @@
       <c r="J6" t="s">
         <v>20</v>
       </c>
+      <c r="K6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1043,6 +1052,178 @@
       </c>
       <c r="K8" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>28252</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>223</v>
+      </c>
+      <c r="G9">
+        <v>111</v>
+      </c>
+      <c r="H9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2222</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10">
+        <v>1111</v>
+      </c>
+      <c r="E10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10">
+        <v>223</v>
+      </c>
+      <c r="G10">
+        <v>111</v>
+      </c>
+      <c r="H10" t="s">
+        <v>24</v>
+      </c>
+      <c r="I10" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" t="s">
+        <v>20</v>
+      </c>
+      <c r="K10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11">
+        <v>223</v>
+      </c>
+      <c r="G11">
+        <v>111</v>
+      </c>
+      <c r="H11" t="s">
+        <v>24</v>
+      </c>
+      <c r="I11" t="s">
+        <v>19</v>
+      </c>
+      <c r="J11" t="s">
+        <v>20</v>
+      </c>
+      <c r="K11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>111</v>
+      </c>
+      <c r="H12" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>555</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13">
+        <v>11</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>435345</v>
+      </c>
+      <c r="H13" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update unit est for add cage and add bird
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACF9450-88BB-4BF1-9D81-C96A9BF39930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9782719F-52AF-4C9D-9817-4BB8A7501E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2088" yWindow="0" windowWidth="11520" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -136,12 +136,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -159,12 +165,14 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,59 +765,61 @@
   <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.8984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>111</v>
       </c>
@@ -819,22 +829,22 @@
       <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>99</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>45061</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -844,7 +854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>223</v>
       </c>
@@ -854,22 +864,22 @@
       <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>99</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>45061</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J3" s="1" t="s">
@@ -879,20 +889,20 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>1231</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="1">
@@ -901,191 +911,191 @@
       <c r="G4" s="1">
         <v>111</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="H4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K4" t="s">
+      <c r="K4" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>435345</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="1">
         <v>223</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="1">
         <v>111</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K5" t="s">
+      <c r="K5" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>534534</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="1">
         <v>223</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="1">
         <v>435345</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>432423</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="1">
         <v>223</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="1">
         <v>111</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K7" t="s">
+      <c r="K7" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>101</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="1">
         <v>223</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="1">
         <v>111</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K8" t="s">
+      <c r="K8" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>207338351</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="1">
         <v>223</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="1">
         <v>435345</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cage and checkmark working for all
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD06B64-E7D4-4838-A055-77C3BC58C1BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0954C9CC-3614-4922-B46C-29BDDA1E2FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72" yWindow="336" windowWidth="11976" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2088" yWindow="0" windowWidth="11520" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="32">
   <si>
     <t>CageID</t>
   </si>
@@ -762,7 +762,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
@@ -1169,6 +1169,73 @@
         <v>25</v>
       </c>
     </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>13215132352</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>223</v>
+      </c>
+      <c r="G12" s="1">
+        <v>534534</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1321513235211</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1">
+        <v>223</v>
+      </c>
+      <c r="G13" s="1">
+        <v>207338351</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">

</xml_diff>

<commit_message>
another database changes take this version
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76DA525F-7D5C-4E02-A930-C1657F655A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7420BB-0C2E-4676-8E1D-29F1A150367F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
   <si>
     <t>CageID</t>
   </si>
@@ -762,15 +762,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.796875" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.09765625" style="1" customWidth="1"/>
     <col min="3" max="3" width="23.19921875" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.8984375" style="1" customWidth="1"/>
@@ -1169,76 +1169,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>13215132352</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="1">
-        <v>223</v>
-      </c>
-      <c r="G12" s="1">
-        <v>534534</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1321513235211</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" s="1">
-        <v>223</v>
-      </c>
-      <c r="G13" s="1">
-        <v>207338351</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
   </sheetData>
   <conditionalFormatting sqref="J2">
     <cfRule type="cellIs" dxfId="43" priority="34" operator="equal">

</xml_diff>

<commit_message>
bug fixed and update icons for project
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7420BB-0C2E-4676-8E1D-29F1A150367F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CF09A5-BEE2-42AD-AF1E-DA9491B42020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3765" yWindow="1305" windowWidth="30255" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="36">
   <si>
     <t>CageID</t>
   </si>
@@ -121,6 +121,18 @@
   </si>
   <si>
     <t>White Pastel</t>
+  </si>
+  <si>
+    <t>22A</t>
+  </si>
+  <si>
+    <t>Central America</t>
+  </si>
+  <si>
+    <t>18/05/2023</t>
+  </si>
+  <si>
+    <t>Green Pastel</t>
   </si>
 </sst>
 </file>
@@ -762,29 +774,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.796875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="26.09765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23.19921875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.8984375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.8984375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="9.59765625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="19.75" style="1" customWidth="1"/>
+    <col min="2" max="2" width="26.125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="23.25" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="10" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.69921875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.75" style="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.59765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.19921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.25" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -819,7 +831,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>111</v>
       </c>
@@ -830,7 +842,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>12</v>
@@ -854,7 +866,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>223</v>
       </c>
@@ -889,7 +901,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>1231</v>
       </c>
@@ -924,7 +936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>435345</v>
       </c>
@@ -959,7 +971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>534534</v>
       </c>
@@ -994,7 +1006,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>432423</v>
       </c>
@@ -1029,7 +1041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>101</v>
       </c>
@@ -1064,7 +1076,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>207338351</v>
       </c>
@@ -1099,7 +1111,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>318692993</v>
       </c>
@@ -1134,7 +1146,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>111111</v>
       </c>
@@ -1167,6 +1179,146 @@
       </c>
       <c r="K11" s="1" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>54332</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="1">
+        <v>223</v>
+      </c>
+      <c r="G12" s="1">
+        <v>111</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>543322</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="1">
+        <v>223</v>
+      </c>
+      <c r="G13" s="1">
+        <v>111</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>3425</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="1">
+        <v>101</v>
+      </c>
+      <c r="G14" s="1">
+        <v>1231</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>222</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="1">
+        <v>444</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1">
+        <v>101</v>
+      </c>
+      <c r="G15" s="1">
+        <v>1231</v>
+      </c>
+      <c r="H15" s="2">
+        <v>45144</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bugs : limit bird date
</commit_message>
<xml_diff>
--- a/DataBased/BirdDB.xlsx
+++ b/DataBased/BirdDB.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\FeatherFriend\DataBased\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8117C24-DBEB-4B27-98B8-9E8904268DE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDDD635-0407-4833-99A6-D1C61C05BBAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3765" yWindow="1305" windowWidth="30255" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="39">
   <si>
     <t>CageID</t>
   </si>
@@ -139,6 +139,9 @@
   </si>
   <si>
     <t>343f</t>
+  </si>
+  <si>
+    <t>גד</t>
   </si>
 </sst>
 </file>
@@ -780,7 +783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
@@ -883,7 +886,7 @@
         <v>17</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
@@ -952,8 +955,8 @@
       <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>26</v>
+      <c r="D5" s="1">
+        <v>32</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>12</v>
@@ -1394,6 +1397,41 @@
         <v>20</v>
       </c>
       <c r="K17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1">
+        <v>32</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="1">
+        <v>318692993</v>
+      </c>
+      <c r="G18" s="1">
+        <v>435345</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K18" s="1" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>